<commit_message>
Envoi de la lettre d'informations et amélioration du site
</commit_message>
<xml_diff>
--- a/doc/amelioration soamada.xlsx
+++ b/doc/amelioration soamada.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="576" yWindow="36" windowWidth="17064" windowHeight="7176"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="test_05042019" sheetId="1" r:id="rId1"/>
+    <sheet name="test_09042019" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Onglets projets liste déroulante</t>
   </si>
@@ -30,12 +30,6 @@
     <t>Menu centré</t>
   </si>
   <si>
-    <t>Mettre les champs obligatoires au début du formulaire enregistrement avant le refresh</t>
-  </si>
-  <si>
-    <t>Ajax</t>
-  </si>
-  <si>
     <t>Connecté avec Facebook</t>
   </si>
   <si>
@@ -52,6 +46,48 @@
   </si>
   <si>
     <t>API s'inscrire avec Facebook et Google</t>
+  </si>
+  <si>
+    <t>Avis Elie</t>
+  </si>
+  <si>
+    <t>Commentaire Ruben</t>
+  </si>
+  <si>
+    <t>Décaler l'icone du texte "projet" dans la bare déroulante</t>
+  </si>
+  <si>
+    <t>Commet savoir qu'on est  l'accueil? Mettre "Bienvenue"</t>
+  </si>
+  <si>
+    <t>Changer le format de chaque section (fontaine, cantine…)</t>
+  </si>
+  <si>
+    <t>Changer les images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Envoyer tous les emails sur la boite d'honoré </t>
+  </si>
+  <si>
+    <t>Priorité</t>
+  </si>
+  <si>
+    <t>Mettre les erreurs des champs obligatoires avant le refresh</t>
+  </si>
+  <si>
+    <t>Mettre les erreurs des champs obligatoire en rouge</t>
+  </si>
+  <si>
+    <t>Vérifier le scrolling sur les articles</t>
+  </si>
+  <si>
+    <t>Ajax pour les adresses</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>ajax pour l'affichage des formulaire - ex Koudetat</t>
   </si>
 </sst>
 </file>
@@ -66,12 +102,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,8 +128,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,72 +432,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -464,12 +530,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="47.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.09765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>